<commit_message>
Update 00Consolidado Tablas Madre.xlsx
</commit_message>
<xml_diff>
--- a/00Consolidado Tablas Madre.xlsx
+++ b/00Consolidado Tablas Madre.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="631">
   <si>
     <t>Código Tabla</t>
   </si>
@@ -1925,6 +1925,30 @@
   </si>
   <si>
     <t>Cosecha de especies en centros de acuicultura por especie y por mes año 2019</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Pueblos_Comuna_Edad</t>
+  </si>
+  <si>
+    <t>Persona</t>
+  </si>
+  <si>
+    <t>Indefinido (Decenio)</t>
+  </si>
+  <si>
+    <t>Instituto Nacional de Estadísticas</t>
+  </si>
+  <si>
+    <t>Demografía</t>
+  </si>
+  <si>
+    <t>20.01</t>
+  </si>
+  <si>
+    <t>Pueblos_Comuna_Genero</t>
   </si>
 </sst>
 </file>
@@ -2598,8 +2622,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D17D0E71-BA07-4DA2-B765-A4376FC7396F}" name="Consolidado_Tablas_Madre" displayName="Consolidado_Tablas_Madre" ref="A11:L146" totalsRowShown="0">
-  <autoFilter ref="A11:L146" xr:uid="{333475B6-F6EF-45EB-8173-D80D5B2B00C0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D17D0E71-BA07-4DA2-B765-A4376FC7396F}" name="Consolidado_Tablas_Madre" displayName="Consolidado_Tablas_Madre" ref="A11:L148" totalsRowShown="0">
+  <autoFilter ref="A11:L148" xr:uid="{333475B6-F6EF-45EB-8173-D80D5B2B00C0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:J136">
     <sortCondition ref="A11:A136"/>
   </sortState>
@@ -2918,11 +2942,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD49B1B1-33D3-49D9-BF85-AA2E2407F985}">
-  <dimension ref="A11:L146"/>
+  <dimension ref="A11:L148"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C126" sqref="C126"/>
+      <pane ySplit="11" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A149" sqref="A149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -7803,6 +7827,68 @@
       </c>
       <c r="L146" t="s">
         <v>315</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12">
+      <c r="A147" s="13" t="s">
+        <v>623</v>
+      </c>
+      <c r="B147" t="s">
+        <v>624</v>
+      </c>
+      <c r="D147" t="s">
+        <v>625</v>
+      </c>
+      <c r="E147" t="s">
+        <v>626</v>
+      </c>
+      <c r="F147" t="s">
+        <v>15</v>
+      </c>
+      <c r="G147" t="s">
+        <v>627</v>
+      </c>
+      <c r="H147" s="10"/>
+      <c r="I147" s="1"/>
+      <c r="J147" t="s">
+        <v>536</v>
+      </c>
+      <c r="K147" t="s">
+        <v>30</v>
+      </c>
+      <c r="L147" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12">
+      <c r="A148" s="13" t="s">
+        <v>629</v>
+      </c>
+      <c r="B148" t="s">
+        <v>630</v>
+      </c>
+      <c r="D148" t="s">
+        <v>625</v>
+      </c>
+      <c r="E148" t="s">
+        <v>626</v>
+      </c>
+      <c r="F148" t="s">
+        <v>15</v>
+      </c>
+      <c r="G148" t="s">
+        <v>627</v>
+      </c>
+      <c r="H148" s="1"/>
+      <c r="I148" s="1"/>
+      <c r="J148" t="s">
+        <v>536</v>
+      </c>
+      <c r="K148" t="s">
+        <v>30</v>
+      </c>
+      <c r="L148" t="s">
+        <v>628</v>
       </c>
     </row>
   </sheetData>

</xml_diff>